<commit_message>
SlidingWindow Write Flow was documented
</commit_message>
<xml_diff>
--- a/SlidingWindow.xlsx
+++ b/SlidingWindow.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\compressionProogect\LZ77\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_repos\LZ77\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EDD927-0023-46F4-8FD1-7CD6E7775C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="18240"/>
+    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="21">
   <si>
     <t>a</t>
   </si>
@@ -87,17 +79,26 @@
   </si>
   <si>
     <t>5b</t>
+  </si>
+  <si>
+    <t>triplets</t>
+  </si>
+  <si>
+    <t>Write Flow</t>
+  </si>
+  <si>
+    <t>Triplets</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -105,7 +106,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -160,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -169,11 +177,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,23 +498,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AK42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24:M24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.125" style="2"/>
-    <col min="4" max="17" width="4.625" customWidth="1"/>
-    <col min="18" max="18" width="11.625" customWidth="1"/>
-    <col min="19" max="41" width="4.625" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="4" max="17" width="4.5703125" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" customWidth="1"/>
+    <col min="19" max="41" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -517,7 +528,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -599,15 +610,15 @@
       <c r="AI2" s="1"/>
       <c r="AJ2" s="1"/>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C3" s="2">
         <v>0</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
       <c r="S3" t="s">
         <v>0</v>
       </c>
@@ -645,12 +656,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="S4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AI4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJ4" s="8"/>
+      <c r="AK4" s="8"/>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <v>1</v>
       </c>
@@ -684,9 +700,9 @@
       <c r="M6" t="s">
         <v>0</v>
       </c>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
       <c r="S6" t="s">
         <v>0</v>
       </c>
@@ -723,8 +739,17 @@
       <c r="AD6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
@@ -732,7 +757,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
@@ -741,43 +766,43 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <v>2</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
       <c r="S9" t="s">
         <v>0</v>
       </c>
@@ -814,8 +839,17 @@
       <c r="AD9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AI9">
+        <v>1</v>
+      </c>
+      <c r="AJ9">
+        <v>2</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
@@ -824,7 +858,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
@@ -834,43 +868,43 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <v>3</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="M12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
+      <c r="D12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
       <c r="S12" t="s">
         <v>0</v>
       </c>
@@ -907,8 +941,17 @@
       <c r="AD12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AI12">
+        <v>1</v>
+      </c>
+      <c r="AJ12">
+        <v>2</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>9</v>
       </c>
@@ -920,7 +963,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
         <v>7</v>
       </c>
@@ -933,7 +976,7 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
         <v>12</v>
       </c>
@@ -967,9 +1010,9 @@
       <c r="M15" t="s">
         <v>11</v>
       </c>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
       <c r="S15" t="s">
         <v>0</v>
       </c>
@@ -1007,7 +1050,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
         <v>9</v>
       </c>
@@ -1024,7 +1067,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="3:31" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
         <v>7</v>
       </c>
@@ -1040,45 +1083,45 @@
       <c r="M17" s="3"/>
       <c r="N17" s="4"/>
     </row>
-    <row r="18" spans="3:31" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="L18" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="M18" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="P18" s="6" t="s">
+      <c r="D18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
       <c r="S18" t="s">
         <v>0</v>
       </c>
@@ -1115,8 +1158,17 @@
       <c r="AD18" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="AI18">
+        <v>1</v>
+      </c>
+      <c r="AJ18">
+        <v>1</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C19" s="2" t="s">
         <v>9</v>
       </c>
@@ -1131,7 +1183,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="3:31" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
         <v>7</v>
       </c>
@@ -1147,7 +1199,7 @@
       <c r="M20" s="3"/>
       <c r="N20" s="4"/>
     </row>
-    <row r="21" spans="3:31" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
         <v>10</v>
       </c>
@@ -1181,9 +1233,9 @@
       <c r="M21" t="s">
         <v>11</v>
       </c>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
       <c r="S21" t="s">
         <v>0</v>
       </c>
@@ -1221,7 +1273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="3:31" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
         <v>9</v>
       </c>
@@ -1241,7 +1293,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="3:31" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C23" s="2" t="s">
         <v>7</v>
       </c>
@@ -1258,45 +1310,45 @@
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
     </row>
-    <row r="24" spans="3:31" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J24" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="K24" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="L24" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="M24" s="7" t="s">
+      <c r="D24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M24" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="P24" s="6" t="s">
+      <c r="P24" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
       <c r="S24" t="s">
         <v>0</v>
       </c>
@@ -1333,8 +1385,17 @@
       <c r="AD24" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="AI24">
+        <v>0</v>
+      </c>
+      <c r="AJ24">
+        <v>0</v>
+      </c>
+      <c r="AK24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C25" s="2" t="s">
         <v>9</v>
       </c>
@@ -1352,7 +1413,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="3:31" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
         <v>7</v>
       </c>
@@ -1367,38 +1428,38 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
     </row>
-    <row r="27" spans="3:31" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <v>6</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="L27" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="M27" s="8" t="s">
+      <c r="D27" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="M27" s="7" t="s">
         <v>3</v>
       </c>
       <c r="S27" t="s">
@@ -1437,8 +1498,17 @@
       <c r="AD27" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="AI27">
+        <v>1</v>
+      </c>
+      <c r="AJ27">
+        <v>1</v>
+      </c>
+      <c r="AK27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
         <v>9</v>
       </c>
@@ -1456,7 +1526,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="3:31" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
         <v>7</v>
       </c>
@@ -1471,38 +1541,38 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="3:31" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <v>7</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="I30" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="K30" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="L30" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="M30" s="8" t="s">
+      <c r="D30" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L30" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="M30" s="7" t="s">
         <v>3</v>
       </c>
       <c r="S30" t="s">
@@ -1542,7 +1612,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="3:31" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C31" s="2" t="s">
         <v>9</v>
       </c>
@@ -1560,7 +1630,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="3:31" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C32" s="2" t="s">
         <v>7</v>
       </c>
@@ -1575,8 +1645,227 @@
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
     </row>
+    <row r="36" spans="3:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C36" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="S36" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="T36" s="8"/>
+      <c r="U36" s="8"/>
+    </row>
+    <row r="37" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="D37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="S37">
+        <v>0</v>
+      </c>
+      <c r="T37">
+        <v>0</v>
+      </c>
+      <c r="U37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="D38" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="S38">
+        <v>1</v>
+      </c>
+      <c r="T38">
+        <v>2</v>
+      </c>
+      <c r="U38" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="D39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="S39">
+        <v>1</v>
+      </c>
+      <c r="T39">
+        <v>2</v>
+      </c>
+      <c r="U39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>0</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="S40">
+        <v>1</v>
+      </c>
+      <c r="T40">
+        <v>1</v>
+      </c>
+      <c r="U40" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>0</v>
+      </c>
+      <c r="F41" t="s">
+        <v>0</v>
+      </c>
+      <c r="G41" t="s">
+        <v>1</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L41" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M41" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="S41">
+        <v>0</v>
+      </c>
+      <c r="T41">
+        <v>0</v>
+      </c>
+      <c r="U41" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" t="s">
+        <v>0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>0</v>
+      </c>
+      <c r="G42" t="s">
+        <v>1</v>
+      </c>
+      <c r="H42" t="s">
+        <v>1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>1</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L42" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M42" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="N42" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="O42" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="S42">
+        <v>1</v>
+      </c>
+      <c r="T42">
+        <v>1</v>
+      </c>
+      <c r="U42" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="11">
+    <mergeCell ref="AI4:AK4"/>
+    <mergeCell ref="C36:N36"/>
+    <mergeCell ref="S36:U36"/>
     <mergeCell ref="P21:R21"/>
     <mergeCell ref="P24:R24"/>
     <mergeCell ref="P3:R3"/>

</xml_diff>